<commit_message>
Refined ML Pipeline v1
</commit_message>
<xml_diff>
--- a/data/Cleaned_Bosch_Dataset.xlsx
+++ b/data/Cleaned_Bosch_Dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Downloads\Nonsense3\Nonsense3\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Downloads\Nonsense3\Baddie_Bosch_Backend_ML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264439C4-59FD-4D02-9CB0-037CE0F60A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49004AA-F9C0-4976-9F7F-B5F042EF5B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27543105-21CB-4FC8-B1B2-88C4FC8B3EE5}"/>
   </bookViews>
@@ -2825,14 +2825,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3210,11 +3209,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE2C3EB-A924-461F-9B8B-E7CC2844F9BF}">
   <dimension ref="A1:U162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="Q143" sqref="Q143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10398,11 +10400,11 @@
       <c r="M140">
         <v>1</v>
       </c>
-      <c r="N140" s="4">
+      <c r="N140" s="1">
         <v>45624</v>
       </c>
-      <c r="O140" s="4">
-        <v>45989</v>
+      <c r="O140" s="1">
+        <v>45624</v>
       </c>
       <c r="P140">
         <v>9.1</v>
@@ -10454,11 +10456,11 @@
       <c r="M141">
         <v>1</v>
       </c>
-      <c r="N141" s="4">
+      <c r="N141" s="1">
         <v>45624</v>
       </c>
-      <c r="O141" s="4">
-        <v>45989</v>
+      <c r="O141" s="1">
+        <v>45624</v>
       </c>
       <c r="P141">
         <v>9.1</v>
@@ -10510,11 +10512,11 @@
       <c r="M142">
         <v>1</v>
       </c>
-      <c r="N142" s="4">
+      <c r="N142" s="1">
         <v>45624</v>
       </c>
-      <c r="O142" s="4">
-        <v>45989</v>
+      <c r="O142" s="1">
+        <v>45624</v>
       </c>
       <c r="P142">
         <v>9.1</v>
@@ -10566,11 +10568,11 @@
       <c r="M143">
         <v>1</v>
       </c>
-      <c r="N143" s="4">
+      <c r="N143" s="1">
         <v>45624</v>
       </c>
-      <c r="O143" s="4">
-        <v>45989</v>
+      <c r="O143" s="1">
+        <v>45624</v>
       </c>
       <c r="P143">
         <v>9.1</v>
@@ -10622,11 +10624,11 @@
       <c r="M144">
         <v>1</v>
       </c>
-      <c r="N144" s="4">
+      <c r="N144" s="1">
         <v>45624</v>
       </c>
-      <c r="O144" s="4">
-        <v>45989</v>
+      <c r="O144" s="1">
+        <v>45624</v>
       </c>
       <c r="P144">
         <v>9.1</v>
@@ -10678,11 +10680,11 @@
       <c r="M145">
         <v>1</v>
       </c>
-      <c r="N145" s="4">
+      <c r="N145" s="1">
         <v>45624</v>
       </c>
-      <c r="O145" s="4">
-        <v>45989</v>
+      <c r="O145" s="1">
+        <v>45624</v>
       </c>
       <c r="P145">
         <v>9.1</v>

</xml_diff>